<commit_message>
Add Dominant Active-catenin diffex
See #1.
</commit_message>
<xml_diff>
--- a/data/filtered.xlsx
+++ b/data/filtered.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="45">
   <si>
     <t>name_a</t>
   </si>
@@ -33,10 +33,16 @@
     <t>endo_fc_a</t>
   </si>
   <si>
+    <t>dac_fc_a</t>
+  </si>
+  <si>
     <t>opc_fc_b</t>
   </si>
   <si>
     <t>endo_fc_b</t>
+  </si>
+  <si>
+    <t>dac_fc_b</t>
   </si>
   <si>
     <t>Alcam</t>
@@ -502,13 +508,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G101"/>
+  <dimension ref="A1:I101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -530,13 +536,19 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:7">
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C2">
         <v>858</v>
@@ -547,19 +559,19 @@
       <c r="E2">
         <v>-3.5519</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>1.075</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <v>2.3607</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:9">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C3">
         <v>900</v>
@@ -570,19 +582,19 @@
       <c r="E3">
         <v>5.4665</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>2.1161</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>-3.946</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:9">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C4">
         <v>901</v>
@@ -593,19 +605,19 @@
       <c r="E4">
         <v>5.4665</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>1.5265</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>1.4406</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:9">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C5">
         <v>903</v>
@@ -616,19 +628,22 @@
       <c r="E5">
         <v>5.4665</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <v>1.1729</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <v>2.7818</v>
       </c>
-    </row>
-    <row r="6" spans="1:7">
+      <c r="I5">
+        <v>1.1388</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C6">
         <v>705</v>
@@ -639,19 +654,19 @@
       <c r="E6">
         <v>5.4665</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <v>0</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <v>2.4959</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:9">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C7">
         <v>993</v>
@@ -662,19 +677,19 @@
       <c r="E7">
         <v>1.6164</v>
       </c>
-      <c r="F7">
+      <c r="G7">
         <v>2.0542</v>
       </c>
-      <c r="G7">
+      <c r="H7">
         <v>1.421</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:9">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C8">
         <v>945</v>
@@ -685,19 +700,19 @@
       <c r="E8">
         <v>1.6164</v>
       </c>
-      <c r="F8">
+      <c r="G8">
         <v>4.1105</v>
       </c>
-      <c r="G8">
+      <c r="H8">
         <v>0.87557</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:9">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B9" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C9">
         <v>782</v>
@@ -708,19 +723,19 @@
       <c r="E9">
         <v>1.6164</v>
       </c>
-      <c r="F9">
+      <c r="G9">
         <v>3.9704</v>
       </c>
-      <c r="G9">
+      <c r="H9">
         <v>-2.8994</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:9">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B10" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C10">
         <v>730</v>
@@ -731,19 +746,19 @@
       <c r="E10">
         <v>1.6164</v>
       </c>
-      <c r="F10">
+      <c r="G10">
         <v>3.7681</v>
       </c>
-      <c r="G10">
+      <c r="H10">
         <v>-3.7786</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:9">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C11">
         <v>904</v>
@@ -754,19 +769,19 @@
       <c r="E11">
         <v>1.6164</v>
       </c>
-      <c r="F11">
+      <c r="G11">
         <v>4.8533</v>
       </c>
-      <c r="G11">
+      <c r="H11">
         <v>-2.634</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:9">
       <c r="A12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" t="s">
         <v>10</v>
-      </c>
-      <c r="B12" t="s">
-        <v>8</v>
       </c>
       <c r="C12">
         <v>900</v>
@@ -777,19 +792,19 @@
       <c r="E12">
         <v>-3.946</v>
       </c>
-      <c r="F12">
+      <c r="G12">
         <v>2.6875</v>
       </c>
-      <c r="G12">
+      <c r="H12">
         <v>5.4665</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:9">
       <c r="A13" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C13">
         <v>909</v>
@@ -800,19 +815,22 @@
       <c r="E13">
         <v>-3.946</v>
       </c>
-      <c r="F13">
+      <c r="G13">
         <v>1.1729</v>
       </c>
-      <c r="G13">
+      <c r="H13">
         <v>2.7818</v>
       </c>
-    </row>
-    <row r="14" spans="1:7">
+      <c r="I13">
+        <v>1.1388</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
       <c r="A14" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C14">
         <v>728</v>
@@ -823,19 +841,19 @@
       <c r="E14">
         <v>-3.946</v>
       </c>
-      <c r="F14">
+      <c r="G14">
         <v>0</v>
       </c>
-      <c r="G14">
+      <c r="H14">
         <v>2.4959</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:9">
       <c r="A15" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B15" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C15">
         <v>710</v>
@@ -846,19 +864,19 @@
       <c r="E15">
         <v>-3.946</v>
       </c>
-      <c r="F15">
+      <c r="G15">
         <v>1.2682</v>
       </c>
-      <c r="G15">
+      <c r="H15">
         <v>6.8898</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:9">
       <c r="A16" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" t="s">
         <v>11</v>
-      </c>
-      <c r="B16" t="s">
-        <v>9</v>
       </c>
       <c r="C16">
         <v>993</v>
@@ -869,19 +887,19 @@
       <c r="E16">
         <v>1.421</v>
       </c>
-      <c r="F16">
+      <c r="G16">
         <v>2.7299</v>
       </c>
-      <c r="G16">
+      <c r="H16">
         <v>1.6164</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:9">
       <c r="A17" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B17" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C17">
         <v>901</v>
@@ -892,19 +910,19 @@
       <c r="E17">
         <v>1.4406</v>
       </c>
-      <c r="F17">
+      <c r="G17">
         <v>2.6875</v>
       </c>
-      <c r="G17">
+      <c r="H17">
         <v>5.4665</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:9">
       <c r="A18" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B18" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C18">
         <v>999</v>
@@ -915,19 +933,22 @@
       <c r="E18">
         <v>1.4406</v>
       </c>
-      <c r="F18">
+      <c r="G18">
         <v>1.1729</v>
       </c>
-      <c r="G18">
+      <c r="H18">
         <v>2.7818</v>
       </c>
-    </row>
-    <row r="19" spans="1:7">
+      <c r="I18">
+        <v>1.1388</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
       <c r="A19" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B19" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C19">
         <v>753</v>
@@ -938,19 +959,19 @@
       <c r="E19">
         <v>1.4406</v>
       </c>
-      <c r="F19">
+      <c r="G19">
         <v>0</v>
       </c>
-      <c r="G19">
+      <c r="H19">
         <v>2.4959</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:9">
       <c r="A20" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B20" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C20">
         <v>718</v>
@@ -961,19 +982,19 @@
       <c r="E20">
         <v>1.4406</v>
       </c>
-      <c r="F20">
+      <c r="G20">
         <v>1.2682</v>
       </c>
-      <c r="G20">
+      <c r="H20">
         <v>6.8898</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:9">
       <c r="A21" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B21" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C21">
         <v>903</v>
@@ -985,18 +1006,21 @@
         <v>2.7818</v>
       </c>
       <c r="F21">
+        <v>1.1388</v>
+      </c>
+      <c r="G21">
         <v>2.6875</v>
       </c>
-      <c r="G21">
+      <c r="H21">
         <v>5.4665</v>
       </c>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:9">
       <c r="A22" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B22" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C22">
         <v>909</v>
@@ -1008,18 +1032,21 @@
         <v>2.7818</v>
       </c>
       <c r="F22">
+        <v>1.1388</v>
+      </c>
+      <c r="G22">
         <v>2.1161</v>
       </c>
-      <c r="G22">
+      <c r="H22">
         <v>-3.946</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:9">
       <c r="A23" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B23" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C23">
         <v>999</v>
@@ -1031,18 +1058,21 @@
         <v>2.7818</v>
       </c>
       <c r="F23">
+        <v>1.1388</v>
+      </c>
+      <c r="G23">
         <v>1.5265</v>
       </c>
-      <c r="G23">
+      <c r="H23">
         <v>1.4406</v>
       </c>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:9">
       <c r="A24" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B24" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C24">
         <v>870</v>
@@ -1054,18 +1084,21 @@
         <v>2.7818</v>
       </c>
       <c r="F24">
+        <v>1.1388</v>
+      </c>
+      <c r="G24">
         <v>3.7681</v>
       </c>
-      <c r="G24">
+      <c r="H24">
         <v>-3.7786</v>
       </c>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:9">
       <c r="A25" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B25" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C25">
         <v>749</v>
@@ -1076,19 +1109,19 @@
       <c r="E25">
         <v>6.2643</v>
       </c>
-      <c r="F25">
+      <c r="G25">
         <v>3.9704</v>
       </c>
-      <c r="G25">
+      <c r="H25">
         <v>-2.8994</v>
       </c>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:9">
       <c r="A26" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B26" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C26">
         <v>945</v>
@@ -1099,19 +1132,19 @@
       <c r="E26">
         <v>0.87557</v>
       </c>
-      <c r="F26">
+      <c r="G26">
         <v>2.7299</v>
       </c>
-      <c r="G26">
+      <c r="H26">
         <v>1.6164</v>
       </c>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:9">
       <c r="A27" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B27" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C27">
         <v>717</v>
@@ -1122,19 +1155,19 @@
       <c r="E27">
         <v>0.87557</v>
       </c>
-      <c r="F27">
+      <c r="G27">
         <v>2.0042</v>
       </c>
-      <c r="G27">
+      <c r="H27">
         <v>3.0428</v>
       </c>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:9">
       <c r="A28" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B28" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C28">
         <v>848</v>
@@ -1145,19 +1178,19 @@
       <c r="E28">
         <v>0.87557</v>
       </c>
-      <c r="F28">
+      <c r="G28">
         <v>0</v>
       </c>
-      <c r="G28">
+      <c r="H28">
         <v>2.4959</v>
       </c>
     </row>
-    <row r="29" spans="1:7">
+    <row r="29" spans="1:9">
       <c r="A29" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B29" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C29">
         <v>876</v>
@@ -1168,19 +1201,19 @@
       <c r="E29">
         <v>0.87557</v>
       </c>
-      <c r="F29">
+      <c r="G29">
         <v>1.2682</v>
       </c>
-      <c r="G29">
+      <c r="H29">
         <v>6.8898</v>
       </c>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:9">
       <c r="A30" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B30" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C30">
         <v>756</v>
@@ -1191,19 +1224,19 @@
       <c r="E30">
         <v>0.87557</v>
       </c>
-      <c r="F30">
+      <c r="G30">
         <v>2.8</v>
       </c>
-      <c r="G30">
+      <c r="H30">
         <v>1.9638</v>
       </c>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="1:9">
       <c r="A31" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B31" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C31">
         <v>846</v>
@@ -1214,19 +1247,19 @@
       <c r="E31">
         <v>0.87557</v>
       </c>
-      <c r="F31">
+      <c r="G31">
         <v>1.075</v>
       </c>
-      <c r="G31">
+      <c r="H31">
         <v>2.3607</v>
       </c>
     </row>
-    <row r="32" spans="1:7">
+    <row r="32" spans="1:9">
       <c r="A32" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B32" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C32">
         <v>863</v>
@@ -1237,19 +1270,19 @@
       <c r="E32">
         <v>0.87557</v>
       </c>
-      <c r="F32">
+      <c r="G32">
         <v>0</v>
       </c>
-      <c r="G32">
+      <c r="H32">
         <v>3.4014</v>
       </c>
     </row>
-    <row r="33" spans="1:7">
+    <row r="33" spans="1:8">
       <c r="A33" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B33" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C33">
         <v>717</v>
@@ -1260,19 +1293,19 @@
       <c r="E33">
         <v>3.0428</v>
       </c>
-      <c r="F33">
+      <c r="G33">
         <v>4.1105</v>
       </c>
-      <c r="G33">
+      <c r="H33">
         <v>0.87557</v>
       </c>
     </row>
-    <row r="34" spans="1:7">
+    <row r="34" spans="1:8">
       <c r="A34" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B34" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C34">
         <v>780</v>
@@ -1283,19 +1316,19 @@
       <c r="E34">
         <v>3.0428</v>
       </c>
-      <c r="F34">
+      <c r="G34">
         <v>0</v>
       </c>
-      <c r="G34">
+      <c r="H34">
         <v>2.4959</v>
       </c>
     </row>
-    <row r="35" spans="1:7">
+    <row r="35" spans="1:8">
       <c r="A35" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B35" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C35">
         <v>813</v>
@@ -1306,19 +1339,19 @@
       <c r="E35">
         <v>3.0428</v>
       </c>
-      <c r="F35">
+      <c r="G35">
         <v>3.0818</v>
       </c>
-      <c r="G35">
+      <c r="H35">
         <v>-3.38</v>
       </c>
     </row>
-    <row r="36" spans="1:7">
+    <row r="36" spans="1:8">
       <c r="A36" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B36" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C36">
         <v>705</v>
@@ -1329,19 +1362,19 @@
       <c r="E36">
         <v>2.4959</v>
       </c>
-      <c r="F36">
+      <c r="G36">
         <v>2.6875</v>
       </c>
-      <c r="G36">
+      <c r="H36">
         <v>5.4665</v>
       </c>
     </row>
-    <row r="37" spans="1:7">
+    <row r="37" spans="1:8">
       <c r="A37" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B37" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C37">
         <v>728</v>
@@ -1352,19 +1385,19 @@
       <c r="E37">
         <v>2.4959</v>
       </c>
-      <c r="F37">
+      <c r="G37">
         <v>2.1161</v>
       </c>
-      <c r="G37">
+      <c r="H37">
         <v>-3.946</v>
       </c>
     </row>
-    <row r="38" spans="1:7">
+    <row r="38" spans="1:8">
       <c r="A38" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B38" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C38">
         <v>753</v>
@@ -1375,19 +1408,19 @@
       <c r="E38">
         <v>2.4959</v>
       </c>
-      <c r="F38">
+      <c r="G38">
         <v>1.5265</v>
       </c>
-      <c r="G38">
+      <c r="H38">
         <v>1.4406</v>
       </c>
     </row>
-    <row r="39" spans="1:7">
+    <row r="39" spans="1:8">
       <c r="A39" t="s">
+        <v>19</v>
+      </c>
+      <c r="B39" t="s">
         <v>17</v>
-      </c>
-      <c r="B39" t="s">
-        <v>15</v>
       </c>
       <c r="C39">
         <v>848</v>
@@ -1398,19 +1431,19 @@
       <c r="E39">
         <v>2.4959</v>
       </c>
-      <c r="F39">
+      <c r="G39">
         <v>4.1105</v>
       </c>
-      <c r="G39">
+      <c r="H39">
         <v>0.87557</v>
       </c>
     </row>
-    <row r="40" spans="1:7">
+    <row r="40" spans="1:8">
       <c r="A40" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B40" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C40">
         <v>780</v>
@@ -1421,19 +1454,19 @@
       <c r="E40">
         <v>2.4959</v>
       </c>
-      <c r="F40">
+      <c r="G40">
         <v>2.0042</v>
       </c>
-      <c r="G40">
+      <c r="H40">
         <v>3.0428</v>
       </c>
     </row>
-    <row r="41" spans="1:7">
+    <row r="41" spans="1:8">
       <c r="A41" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B41" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C41">
         <v>829</v>
@@ -1444,19 +1477,19 @@
       <c r="E41">
         <v>2.4959</v>
       </c>
-      <c r="F41">
+      <c r="G41">
         <v>3.0818</v>
       </c>
-      <c r="G41">
+      <c r="H41">
         <v>-3.38</v>
       </c>
     </row>
-    <row r="42" spans="1:7">
+    <row r="42" spans="1:8">
       <c r="A42" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B42" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C42">
         <v>748</v>
@@ -1467,19 +1500,19 @@
       <c r="E42">
         <v>2.4959</v>
       </c>
-      <c r="F42">
+      <c r="G42">
         <v>3.9704</v>
       </c>
-      <c r="G42">
+      <c r="H42">
         <v>-2.8994</v>
       </c>
     </row>
-    <row r="43" spans="1:7">
+    <row r="43" spans="1:8">
       <c r="A43" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B43" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C43">
         <v>804</v>
@@ -1490,19 +1523,19 @@
       <c r="E43">
         <v>2.4959</v>
       </c>
-      <c r="F43">
+      <c r="G43">
         <v>2.9286</v>
       </c>
-      <c r="G43">
+      <c r="H43">
         <v>0.044873</v>
       </c>
     </row>
-    <row r="44" spans="1:7">
+    <row r="44" spans="1:8">
       <c r="A44" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B44" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C44">
         <v>764</v>
@@ -1513,19 +1546,19 @@
       <c r="E44">
         <v>2.4959</v>
       </c>
-      <c r="F44">
+      <c r="G44">
         <v>3.7681</v>
       </c>
-      <c r="G44">
+      <c r="H44">
         <v>-3.7786</v>
       </c>
     </row>
-    <row r="45" spans="1:7">
+    <row r="45" spans="1:8">
       <c r="A45" t="s">
+        <v>20</v>
+      </c>
+      <c r="B45" t="s">
         <v>18</v>
-      </c>
-      <c r="B45" t="s">
-        <v>16</v>
       </c>
       <c r="C45">
         <v>813</v>
@@ -1536,19 +1569,19 @@
       <c r="E45">
         <v>-3.38</v>
       </c>
-      <c r="F45">
+      <c r="G45">
         <v>2.0042</v>
       </c>
-      <c r="G45">
+      <c r="H45">
         <v>3.0428</v>
       </c>
     </row>
-    <row r="46" spans="1:7">
+    <row r="46" spans="1:8">
       <c r="A46" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B46" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C46">
         <v>829</v>
@@ -1559,19 +1592,19 @@
       <c r="E46">
         <v>-3.38</v>
       </c>
-      <c r="F46">
+      <c r="G46">
         <v>0</v>
       </c>
-      <c r="G46">
+      <c r="H46">
         <v>2.4959</v>
       </c>
     </row>
-    <row r="47" spans="1:7">
+    <row r="47" spans="1:8">
       <c r="A47" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B47" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C47">
         <v>710</v>
@@ -1582,19 +1615,19 @@
       <c r="E47">
         <v>6.8898</v>
       </c>
-      <c r="F47">
+      <c r="G47">
         <v>2.1161</v>
       </c>
-      <c r="G47">
+      <c r="H47">
         <v>-3.946</v>
       </c>
     </row>
-    <row r="48" spans="1:7">
+    <row r="48" spans="1:8">
       <c r="A48" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B48" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C48">
         <v>718</v>
@@ -1605,19 +1638,19 @@
       <c r="E48">
         <v>6.8898</v>
       </c>
-      <c r="F48">
+      <c r="G48">
         <v>1.5265</v>
       </c>
-      <c r="G48">
+      <c r="H48">
         <v>1.4406</v>
       </c>
     </row>
-    <row r="49" spans="1:7">
+    <row r="49" spans="1:8">
       <c r="A49" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B49" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C49">
         <v>876</v>
@@ -1628,19 +1661,19 @@
       <c r="E49">
         <v>6.8898</v>
       </c>
-      <c r="F49">
+      <c r="G49">
         <v>4.1105</v>
       </c>
-      <c r="G49">
+      <c r="H49">
         <v>0.87557</v>
       </c>
     </row>
-    <row r="50" spans="1:7">
+    <row r="50" spans="1:8">
       <c r="A50" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B50" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C50">
         <v>977</v>
@@ -1651,19 +1684,19 @@
       <c r="E50">
         <v>6.8898</v>
       </c>
-      <c r="F50">
+      <c r="G50">
         <v>2.6682</v>
       </c>
-      <c r="G50">
+      <c r="H50">
         <v>-5.1088</v>
       </c>
     </row>
-    <row r="51" spans="1:7">
+    <row r="51" spans="1:8">
       <c r="A51" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B51" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C51">
         <v>754</v>
@@ -1674,19 +1707,19 @@
       <c r="E51">
         <v>6.8898</v>
       </c>
-      <c r="F51">
+      <c r="G51">
         <v>4.101</v>
       </c>
-      <c r="G51">
+      <c r="H51">
         <v>0.75699</v>
       </c>
     </row>
-    <row r="52" spans="1:7">
+    <row r="52" spans="1:8">
       <c r="A52" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B52" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C52">
         <v>774</v>
@@ -1697,19 +1730,19 @@
       <c r="E52">
         <v>6.8898</v>
       </c>
-      <c r="F52">
+      <c r="G52">
         <v>3.9704</v>
       </c>
-      <c r="G52">
+      <c r="H52">
         <v>-2.8994</v>
       </c>
     </row>
-    <row r="53" spans="1:7">
+    <row r="53" spans="1:8">
       <c r="A53" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B53" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C53">
         <v>732</v>
@@ -1720,19 +1753,19 @@
       <c r="E53">
         <v>6.8898</v>
       </c>
-      <c r="F53">
+      <c r="G53">
         <v>3.7681</v>
       </c>
-      <c r="G53">
+      <c r="H53">
         <v>-3.7786</v>
       </c>
     </row>
-    <row r="54" spans="1:7">
+    <row r="54" spans="1:8">
       <c r="A54" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B54" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C54">
         <v>975</v>
@@ -1743,19 +1776,19 @@
       <c r="E54">
         <v>6.8898</v>
       </c>
-      <c r="F54">
+      <c r="G54">
         <v>4.8533</v>
       </c>
-      <c r="G54">
+      <c r="H54">
         <v>-2.634</v>
       </c>
     </row>
-    <row r="55" spans="1:7">
+    <row r="55" spans="1:8">
       <c r="A55" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B55" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C55">
         <v>756</v>
@@ -1766,19 +1799,19 @@
       <c r="E55">
         <v>1.9638</v>
       </c>
-      <c r="F55">
+      <c r="G55">
         <v>4.1105</v>
       </c>
-      <c r="G55">
+      <c r="H55">
         <v>0.87557</v>
       </c>
     </row>
-    <row r="56" spans="1:7">
+    <row r="56" spans="1:8">
       <c r="A56" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B56" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C56">
         <v>807</v>
@@ -1789,19 +1822,19 @@
       <c r="E56">
         <v>1.9638</v>
       </c>
-      <c r="F56">
+      <c r="G56">
         <v>1.5418</v>
       </c>
-      <c r="G56">
+      <c r="H56">
         <v>-2.0723</v>
       </c>
     </row>
-    <row r="57" spans="1:7">
+    <row r="57" spans="1:8">
       <c r="A57" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B57" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C57">
         <v>999</v>
@@ -1812,19 +1845,19 @@
       <c r="E57">
         <v>1.9638</v>
       </c>
-      <c r="F57">
+      <c r="G57">
         <v>1.075</v>
       </c>
-      <c r="G57">
+      <c r="H57">
         <v>2.3607</v>
       </c>
     </row>
-    <row r="58" spans="1:7">
+    <row r="58" spans="1:8">
       <c r="A58" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B58" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C58">
         <v>961</v>
@@ -1835,19 +1868,19 @@
       <c r="E58">
         <v>1.9638</v>
       </c>
-      <c r="F58">
+      <c r="G58">
         <v>2.6682</v>
       </c>
-      <c r="G58">
+      <c r="H58">
         <v>-5.1088</v>
       </c>
     </row>
-    <row r="59" spans="1:7">
+    <row r="59" spans="1:8">
       <c r="A59" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B59" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C59">
         <v>998</v>
@@ -1858,19 +1891,19 @@
       <c r="E59">
         <v>0.95214</v>
       </c>
-      <c r="F59">
+      <c r="G59">
         <v>1.075</v>
       </c>
-      <c r="G59">
+      <c r="H59">
         <v>2.3607</v>
       </c>
     </row>
-    <row r="60" spans="1:7">
+    <row r="60" spans="1:8">
       <c r="A60" t="s">
+        <v>24</v>
+      </c>
+      <c r="B60" t="s">
         <v>22</v>
-      </c>
-      <c r="B60" t="s">
-        <v>20</v>
       </c>
       <c r="C60">
         <v>807</v>
@@ -1881,19 +1914,19 @@
       <c r="E60">
         <v>-2.0723</v>
       </c>
-      <c r="F60">
+      <c r="G60">
         <v>2.8</v>
       </c>
-      <c r="G60">
+      <c r="H60">
         <v>1.9638</v>
       </c>
     </row>
-    <row r="61" spans="1:7">
+    <row r="61" spans="1:8">
       <c r="A61" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B61" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C61">
         <v>996</v>
@@ -1904,19 +1937,19 @@
       <c r="E61">
         <v>-2.0723</v>
       </c>
-      <c r="F61">
+      <c r="G61">
         <v>1.075</v>
       </c>
-      <c r="G61">
+      <c r="H61">
         <v>2.3607</v>
       </c>
     </row>
-    <row r="62" spans="1:7">
+    <row r="62" spans="1:8">
       <c r="A62" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B62" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C62">
         <v>919</v>
@@ -1927,19 +1960,19 @@
       <c r="E62">
         <v>-8.7568</v>
       </c>
-      <c r="F62">
+      <c r="G62">
         <v>1.075</v>
       </c>
-      <c r="G62">
+      <c r="H62">
         <v>2.3607</v>
       </c>
     </row>
-    <row r="63" spans="1:7">
+    <row r="63" spans="1:8">
       <c r="A63" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B63" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C63">
         <v>931</v>
@@ -1950,19 +1983,19 @@
       <c r="E63">
         <v>-8.7568</v>
       </c>
-      <c r="F63">
+      <c r="G63">
         <v>0</v>
       </c>
-      <c r="G63">
+      <c r="H63">
         <v>3.4014</v>
       </c>
     </row>
-    <row r="64" spans="1:7">
+    <row r="64" spans="1:8">
       <c r="A64" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B64" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C64">
         <v>998</v>
@@ -1973,19 +2006,19 @@
       <c r="E64">
         <v>-2.1728</v>
       </c>
-      <c r="F64">
+      <c r="G64">
         <v>1.075</v>
       </c>
-      <c r="G64">
+      <c r="H64">
         <v>2.3607</v>
       </c>
     </row>
-    <row r="65" spans="1:7">
+    <row r="65" spans="1:8">
       <c r="A65" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B65" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C65">
         <v>858</v>
@@ -1996,19 +2029,19 @@
       <c r="E65">
         <v>2.3607</v>
       </c>
-      <c r="F65">
+      <c r="G65">
         <v>5.5683</v>
       </c>
-      <c r="G65">
+      <c r="H65">
         <v>-3.5519</v>
       </c>
     </row>
-    <row r="66" spans="1:7">
+    <row r="66" spans="1:8">
       <c r="A66" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B66" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C66">
         <v>846</v>
@@ -2019,19 +2052,19 @@
       <c r="E66">
         <v>2.3607</v>
       </c>
-      <c r="F66">
+      <c r="G66">
         <v>4.1105</v>
       </c>
-      <c r="G66">
+      <c r="H66">
         <v>0.87557</v>
       </c>
     </row>
-    <row r="67" spans="1:7">
+    <row r="67" spans="1:8">
       <c r="A67" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B67" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C67">
         <v>999</v>
@@ -2042,19 +2075,19 @@
       <c r="E67">
         <v>2.3607</v>
       </c>
-      <c r="F67">
+      <c r="G67">
         <v>2.8</v>
       </c>
-      <c r="G67">
+      <c r="H67">
         <v>1.9638</v>
       </c>
     </row>
-    <row r="68" spans="1:7">
+    <row r="68" spans="1:8">
       <c r="A68" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B68" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C68">
         <v>998</v>
@@ -2065,19 +2098,19 @@
       <c r="E68">
         <v>2.3607</v>
       </c>
-      <c r="F68">
+      <c r="G68">
         <v>3.6236</v>
       </c>
-      <c r="G68">
+      <c r="H68">
         <v>0.95214</v>
       </c>
     </row>
-    <row r="69" spans="1:7">
+    <row r="69" spans="1:8">
       <c r="A69" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B69" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C69">
         <v>996</v>
@@ -2088,19 +2121,19 @@
       <c r="E69">
         <v>2.3607</v>
       </c>
-      <c r="F69">
+      <c r="G69">
         <v>1.5418</v>
       </c>
-      <c r="G69">
+      <c r="H69">
         <v>-2.0723</v>
       </c>
     </row>
-    <row r="70" spans="1:7">
+    <row r="70" spans="1:8">
       <c r="A70" t="s">
+        <v>27</v>
+      </c>
+      <c r="B70" t="s">
         <v>25</v>
-      </c>
-      <c r="B70" t="s">
-        <v>23</v>
       </c>
       <c r="C70">
         <v>919</v>
@@ -2111,19 +2144,19 @@
       <c r="E70">
         <v>2.3607</v>
       </c>
-      <c r="F70">
+      <c r="G70">
         <v>2.6857</v>
       </c>
-      <c r="G70">
+      <c r="H70">
         <v>-8.7568</v>
       </c>
     </row>
-    <row r="71" spans="1:7">
+    <row r="71" spans="1:8">
       <c r="A71" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B71" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C71">
         <v>998</v>
@@ -2134,19 +2167,19 @@
       <c r="E71">
         <v>2.3607</v>
       </c>
-      <c r="F71">
+      <c r="G71">
         <v>3.7384</v>
       </c>
-      <c r="G71">
+      <c r="H71">
         <v>-2.1728</v>
       </c>
     </row>
-    <row r="72" spans="1:7">
+    <row r="72" spans="1:8">
       <c r="A72" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B72" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C72">
         <v>722</v>
@@ -2157,19 +2190,19 @@
       <c r="E72">
         <v>2.3607</v>
       </c>
-      <c r="F72">
+      <c r="G72">
         <v>4.101</v>
       </c>
-      <c r="G72">
+      <c r="H72">
         <v>0.75699</v>
       </c>
     </row>
-    <row r="73" spans="1:7">
+    <row r="73" spans="1:8">
       <c r="A73" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B73" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C73">
         <v>878</v>
@@ -2180,19 +2213,19 @@
       <c r="E73">
         <v>2.3607</v>
       </c>
-      <c r="F73">
+      <c r="G73">
         <v>2.3859</v>
       </c>
-      <c r="G73">
+      <c r="H73">
         <v>-3.147</v>
       </c>
     </row>
-    <row r="74" spans="1:7">
+    <row r="74" spans="1:8">
       <c r="A74" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B74" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C74">
         <v>942</v>
@@ -2203,19 +2236,19 @@
       <c r="E74">
         <v>2.3607</v>
       </c>
-      <c r="F74">
+      <c r="G74">
         <v>3.9704</v>
       </c>
-      <c r="G74">
+      <c r="H74">
         <v>-2.8994</v>
       </c>
     </row>
-    <row r="75" spans="1:7">
+    <row r="75" spans="1:8">
       <c r="A75" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B75" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C75">
         <v>978</v>
@@ -2226,19 +2259,19 @@
       <c r="E75">
         <v>2.3607</v>
       </c>
-      <c r="F75">
+      <c r="G75">
         <v>4.8533</v>
       </c>
-      <c r="G75">
+      <c r="H75">
         <v>-2.634</v>
       </c>
     </row>
-    <row r="76" spans="1:7">
+    <row r="76" spans="1:8">
       <c r="A76" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B76" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C76">
         <v>977</v>
@@ -2249,19 +2282,19 @@
       <c r="E76">
         <v>-5.1088</v>
       </c>
-      <c r="F76">
+      <c r="G76">
         <v>1.2682</v>
       </c>
-      <c r="G76">
+      <c r="H76">
         <v>6.8898</v>
       </c>
     </row>
-    <row r="77" spans="1:7">
+    <row r="77" spans="1:8">
       <c r="A77" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B77" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C77">
         <v>961</v>
@@ -2272,19 +2305,19 @@
       <c r="E77">
         <v>-5.1088</v>
       </c>
-      <c r="F77">
+      <c r="G77">
         <v>2.8</v>
       </c>
-      <c r="G77">
+      <c r="H77">
         <v>1.9638</v>
       </c>
     </row>
-    <row r="78" spans="1:7">
+    <row r="78" spans="1:8">
       <c r="A78" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B78" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C78">
         <v>887</v>
@@ -2295,19 +2328,19 @@
       <c r="E78">
         <v>-5.1088</v>
       </c>
-      <c r="F78">
+      <c r="G78">
         <v>0</v>
       </c>
-      <c r="G78">
+      <c r="H78">
         <v>3.4014</v>
       </c>
     </row>
-    <row r="79" spans="1:7">
+    <row r="79" spans="1:8">
       <c r="A79" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B79" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C79">
         <v>754</v>
@@ -2318,19 +2351,19 @@
       <c r="E79">
         <v>0.75699</v>
       </c>
-      <c r="F79">
+      <c r="G79">
         <v>1.2682</v>
       </c>
-      <c r="G79">
+      <c r="H79">
         <v>6.8898</v>
       </c>
     </row>
-    <row r="80" spans="1:7">
+    <row r="80" spans="1:8">
       <c r="A80" t="s">
+        <v>29</v>
+      </c>
+      <c r="B80" t="s">
         <v>27</v>
-      </c>
-      <c r="B80" t="s">
-        <v>25</v>
       </c>
       <c r="C80">
         <v>722</v>
@@ -2341,19 +2374,19 @@
       <c r="E80">
         <v>0.75699</v>
       </c>
-      <c r="F80">
+      <c r="G80">
         <v>1.075</v>
       </c>
-      <c r="G80">
+      <c r="H80">
         <v>2.3607</v>
       </c>
     </row>
-    <row r="81" spans="1:7">
+    <row r="81" spans="1:9">
       <c r="A81" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B81" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C81">
         <v>878</v>
@@ -2364,19 +2397,19 @@
       <c r="E81">
         <v>-3.147</v>
       </c>
-      <c r="F81">
+      <c r="G81">
         <v>1.075</v>
       </c>
-      <c r="G81">
+      <c r="H81">
         <v>2.3607</v>
       </c>
     </row>
-    <row r="82" spans="1:7">
+    <row r="82" spans="1:9">
       <c r="A82" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B82" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C82">
         <v>782</v>
@@ -2387,19 +2420,19 @@
       <c r="E82">
         <v>-2.8994</v>
       </c>
-      <c r="F82">
+      <c r="G82">
         <v>2.7299</v>
       </c>
-      <c r="G82">
+      <c r="H82">
         <v>1.6164</v>
       </c>
     </row>
-    <row r="83" spans="1:7">
+    <row r="83" spans="1:9">
       <c r="A83" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B83" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C83">
         <v>749</v>
@@ -2410,19 +2443,19 @@
       <c r="E83">
         <v>-2.8994</v>
       </c>
-      <c r="F83">
+      <c r="G83">
         <v>0.37096</v>
       </c>
-      <c r="G83">
+      <c r="H83">
         <v>6.2643</v>
       </c>
     </row>
-    <row r="84" spans="1:7">
+    <row r="84" spans="1:9">
       <c r="A84" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B84" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C84">
         <v>748</v>
@@ -2433,19 +2466,19 @@
       <c r="E84">
         <v>-2.8994</v>
       </c>
-      <c r="F84">
+      <c r="G84">
         <v>0</v>
       </c>
-      <c r="G84">
+      <c r="H84">
         <v>2.4959</v>
       </c>
     </row>
-    <row r="85" spans="1:7">
+    <row r="85" spans="1:9">
       <c r="A85" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B85" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C85">
         <v>774</v>
@@ -2456,19 +2489,19 @@
       <c r="E85">
         <v>-2.8994</v>
       </c>
-      <c r="F85">
+      <c r="G85">
         <v>1.2682</v>
       </c>
-      <c r="G85">
+      <c r="H85">
         <v>6.8898</v>
       </c>
     </row>
-    <row r="86" spans="1:7">
+    <row r="86" spans="1:9">
       <c r="A86" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B86" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C86">
         <v>942</v>
@@ -2479,19 +2512,19 @@
       <c r="E86">
         <v>-2.8994</v>
       </c>
-      <c r="F86">
+      <c r="G86">
         <v>1.075</v>
       </c>
-      <c r="G86">
+      <c r="H86">
         <v>2.3607</v>
       </c>
     </row>
-    <row r="87" spans="1:7">
+    <row r="87" spans="1:9">
       <c r="A87" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B87" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C87">
         <v>748</v>
@@ -2502,19 +2535,19 @@
       <c r="E87">
         <v>-2.8994</v>
       </c>
-      <c r="F87">
+      <c r="G87">
         <v>1.1988</v>
       </c>
-      <c r="G87">
+      <c r="H87">
         <v>8.6851</v>
       </c>
     </row>
-    <row r="88" spans="1:7">
+    <row r="88" spans="1:9">
       <c r="A88" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B88" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C88">
         <v>863</v>
@@ -2525,19 +2558,19 @@
       <c r="E88">
         <v>3.4014</v>
       </c>
-      <c r="F88">
+      <c r="G88">
         <v>4.1105</v>
       </c>
-      <c r="G88">
+      <c r="H88">
         <v>0.87557</v>
       </c>
     </row>
-    <row r="89" spans="1:7">
+    <row r="89" spans="1:9">
       <c r="A89" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B89" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C89">
         <v>931</v>
@@ -2548,19 +2581,19 @@
       <c r="E89">
         <v>3.4014</v>
       </c>
-      <c r="F89">
+      <c r="G89">
         <v>2.6857</v>
       </c>
-      <c r="G89">
+      <c r="H89">
         <v>-8.7568</v>
       </c>
     </row>
-    <row r="90" spans="1:7">
+    <row r="90" spans="1:9">
       <c r="A90" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B90" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C90">
         <v>887</v>
@@ -2571,19 +2604,19 @@
       <c r="E90">
         <v>3.4014</v>
       </c>
-      <c r="F90">
+      <c r="G90">
         <v>2.6682</v>
       </c>
-      <c r="G90">
+      <c r="H90">
         <v>-5.1088</v>
       </c>
     </row>
-    <row r="91" spans="1:7">
+    <row r="91" spans="1:9">
       <c r="A91" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B91" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C91">
         <v>964</v>
@@ -2594,19 +2627,19 @@
       <c r="E91">
         <v>3.4014</v>
       </c>
-      <c r="F91">
+      <c r="G91">
         <v>3.7681</v>
       </c>
-      <c r="G91">
+      <c r="H91">
         <v>-3.7786</v>
       </c>
     </row>
-    <row r="92" spans="1:7">
+    <row r="92" spans="1:9">
       <c r="A92" t="s">
+        <v>33</v>
+      </c>
+      <c r="B92" t="s">
         <v>31</v>
-      </c>
-      <c r="B92" t="s">
-        <v>29</v>
       </c>
       <c r="C92">
         <v>748</v>
@@ -2617,19 +2650,19 @@
       <c r="E92">
         <v>8.6851</v>
       </c>
-      <c r="F92">
+      <c r="G92">
         <v>3.9704</v>
       </c>
-      <c r="G92">
+      <c r="H92">
         <v>-2.8994</v>
       </c>
     </row>
-    <row r="93" spans="1:7">
+    <row r="93" spans="1:9">
       <c r="A93" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B93" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C93">
         <v>804</v>
@@ -2640,19 +2673,19 @@
       <c r="E93">
         <v>0.044873</v>
       </c>
-      <c r="F93">
+      <c r="G93">
         <v>0</v>
       </c>
-      <c r="G93">
+      <c r="H93">
         <v>2.4959</v>
       </c>
     </row>
-    <row r="94" spans="1:7">
+    <row r="94" spans="1:9">
       <c r="A94" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B94" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C94">
         <v>730</v>
@@ -2663,19 +2696,19 @@
       <c r="E94">
         <v>-3.7786</v>
       </c>
-      <c r="F94">
+      <c r="G94">
         <v>2.7299</v>
       </c>
-      <c r="G94">
+      <c r="H94">
         <v>1.6164</v>
       </c>
     </row>
-    <row r="95" spans="1:7">
+    <row r="95" spans="1:9">
       <c r="A95" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B95" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C95">
         <v>870</v>
@@ -2686,19 +2719,22 @@
       <c r="E95">
         <v>-3.7786</v>
       </c>
-      <c r="F95">
+      <c r="G95">
         <v>1.1729</v>
       </c>
-      <c r="G95">
+      <c r="H95">
         <v>2.7818</v>
       </c>
-    </row>
-    <row r="96" spans="1:7">
+      <c r="I95">
+        <v>1.1388</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9">
       <c r="A96" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B96" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C96">
         <v>764</v>
@@ -2709,19 +2745,19 @@
       <c r="E96">
         <v>-3.7786</v>
       </c>
-      <c r="F96">
+      <c r="G96">
         <v>0</v>
       </c>
-      <c r="G96">
+      <c r="H96">
         <v>2.4959</v>
       </c>
     </row>
-    <row r="97" spans="1:7">
+    <row r="97" spans="1:8">
       <c r="A97" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B97" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C97">
         <v>732</v>
@@ -2732,19 +2768,19 @@
       <c r="E97">
         <v>-3.7786</v>
       </c>
-      <c r="F97">
+      <c r="G97">
         <v>1.2682</v>
       </c>
-      <c r="G97">
+      <c r="H97">
         <v>6.8898</v>
       </c>
     </row>
-    <row r="98" spans="1:7">
+    <row r="98" spans="1:8">
       <c r="A98" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B98" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C98">
         <v>964</v>
@@ -2755,19 +2791,19 @@
       <c r="E98">
         <v>-3.7786</v>
       </c>
-      <c r="F98">
+      <c r="G98">
         <v>0</v>
       </c>
-      <c r="G98">
+      <c r="H98">
         <v>3.4014</v>
       </c>
     </row>
-    <row r="99" spans="1:7">
+    <row r="99" spans="1:8">
       <c r="A99" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B99" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C99">
         <v>904</v>
@@ -2778,19 +2814,19 @@
       <c r="E99">
         <v>-2.634</v>
       </c>
-      <c r="F99">
+      <c r="G99">
         <v>2.7299</v>
       </c>
-      <c r="G99">
+      <c r="H99">
         <v>1.6164</v>
       </c>
     </row>
-    <row r="100" spans="1:7">
+    <row r="100" spans="1:8">
       <c r="A100" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B100" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C100">
         <v>975</v>
@@ -2801,19 +2837,19 @@
       <c r="E100">
         <v>-2.634</v>
       </c>
-      <c r="F100">
+      <c r="G100">
         <v>1.2682</v>
       </c>
-      <c r="G100">
+      <c r="H100">
         <v>6.8898</v>
       </c>
     </row>
-    <row r="101" spans="1:7">
+    <row r="101" spans="1:8">
       <c r="A101" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B101" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C101">
         <v>978</v>
@@ -2824,10 +2860,10 @@
       <c r="E101">
         <v>-2.634</v>
       </c>
-      <c r="F101">
+      <c r="G101">
         <v>1.075</v>
       </c>
-      <c r="G101">
+      <c r="H101">
         <v>2.3607</v>
       </c>
     </row>
@@ -2846,15 +2882,15 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B2">
         <v>22</v>
@@ -2862,7 +2898,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B3">
         <v>18</v>
@@ -2870,7 +2906,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B4">
         <v>16</v>
@@ -2878,7 +2914,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B5">
         <v>14</v>
@@ -2886,7 +2922,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B6">
         <v>12</v>
@@ -2894,7 +2930,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B7">
         <v>10</v>
@@ -2902,7 +2938,7 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B8">
         <v>10</v>
@@ -2910,7 +2946,7 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="B9">
         <v>8</v>
@@ -2918,7 +2954,7 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="B10">
         <v>8</v>
@@ -2934,7 +2970,7 @@
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B12">
         <v>8</v>
@@ -2942,7 +2978,7 @@
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B13">
         <v>8</v>
@@ -2958,7 +2994,7 @@
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>34</v>
+        <v>18</v>
       </c>
       <c r="B15">
         <v>6</v>
@@ -2966,7 +3002,7 @@
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>16</v>
+        <v>36</v>
       </c>
       <c r="B16">
         <v>6</v>
@@ -2974,7 +3010,7 @@
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B17">
         <v>6</v>
@@ -2982,7 +3018,7 @@
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B18">
         <v>4</v>
@@ -2990,7 +3026,7 @@
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="B19">
         <v>4</v>
@@ -2998,7 +3034,7 @@
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B20">
         <v>4</v>
@@ -3006,7 +3042,7 @@
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B21">
         <v>4</v>
@@ -3014,7 +3050,7 @@
     </row>
     <row r="22" spans="1:2">
       <c r="A22" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="B22">
         <v>2</v>
@@ -3022,7 +3058,7 @@
     </row>
     <row r="23" spans="1:2">
       <c r="A23" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="B23">
         <v>2</v>
@@ -3030,7 +3066,7 @@
     </row>
     <row r="24" spans="1:2">
       <c r="A24" t="s">
-        <v>7</v>
+        <v>33</v>
       </c>
       <c r="B24">
         <v>2</v>
@@ -3038,7 +3074,7 @@
     </row>
     <row r="25" spans="1:2">
       <c r="A25" t="s">
-        <v>14</v>
+        <v>30</v>
       </c>
       <c r="B25">
         <v>2</v>
@@ -3046,7 +3082,7 @@
     </row>
     <row r="26" spans="1:2">
       <c r="A26" t="s">
-        <v>31</v>
+        <v>9</v>
       </c>
       <c r="B26">
         <v>2</v>
@@ -3054,7 +3090,7 @@
     </row>
     <row r="27" spans="1:2">
       <c r="A27" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B27">
         <v>2</v>
@@ -3062,7 +3098,7 @@
     </row>
     <row r="28" spans="1:2">
       <c r="A28" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B28">
         <v>2</v>
@@ -3070,7 +3106,7 @@
     </row>
     <row r="29" spans="1:2">
       <c r="A29" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B29">
         <v>2</v>
@@ -3091,15 +3127,15 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B2">
         <v>1.5</v>
@@ -3107,7 +3143,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B3">
         <v>700</v>
@@ -3115,10 +3151,10 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B4" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Specify log2 when referring to fold change
Closes #2.
</commit_message>
<xml_diff>
--- a/data/filtered.xlsx
+++ b/data/filtered.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="41">
   <si>
     <t>name_a</t>
   </si>
@@ -27,22 +27,22 @@
     <t>combined_score</t>
   </si>
   <si>
-    <t>opc_fc_a</t>
-  </si>
-  <si>
-    <t>endo_fc_a</t>
-  </si>
-  <si>
-    <t>dac_fc_a</t>
-  </si>
-  <si>
-    <t>opc_fc_b</t>
-  </si>
-  <si>
-    <t>endo_fc_b</t>
-  </si>
-  <si>
-    <t>dac_fc_b</t>
+    <t>opc_l2fc_a</t>
+  </si>
+  <si>
+    <t>endo_l2fc_a</t>
+  </si>
+  <si>
+    <t>dac_l2fc_a</t>
+  </si>
+  <si>
+    <t>opc_l2fc_b</t>
+  </si>
+  <si>
+    <t>endo_l2fc_b</t>
+  </si>
+  <si>
+    <t>dac_l2fc_b</t>
   </si>
   <si>
     <t>Alcam</t>
@@ -126,7 +126,10 @@
     <t>value</t>
   </si>
   <si>
-    <t>fold_change_cutoff</t>
+    <t>log2_fold_change_cutoff</t>
+  </si>
+  <si>
+    <t>opc_microglia_min_ratio</t>
   </si>
   <si>
     <t>string_score_cutoff</t>
@@ -1967,7 +1970,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="B5">
         <v>8</v>
@@ -1975,7 +1978,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="B6">
         <v>8</v>
@@ -1983,7 +1986,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>31</v>
       </c>
       <c r="B7">
         <v>6</v>
@@ -1991,7 +1994,7 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>31</v>
+        <v>10</v>
       </c>
       <c r="B8">
         <v>6</v>
@@ -1999,7 +2002,7 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B9">
         <v>6</v>
@@ -2007,7 +2010,7 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="B10">
         <v>4</v>
@@ -2015,7 +2018,7 @@
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="B11">
         <v>4</v>
@@ -2023,7 +2026,7 @@
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="B12">
         <v>4</v>
@@ -2031,7 +2034,7 @@
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B13">
         <v>4</v>
@@ -2047,7 +2050,7 @@
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="B15">
         <v>4</v>
@@ -2055,7 +2058,7 @@
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="B16">
         <v>4</v>
@@ -2063,7 +2066,7 @@
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>30</v>
+        <v>9</v>
       </c>
       <c r="B17">
         <v>2</v>
@@ -2071,7 +2074,7 @@
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="B18">
         <v>2</v>
@@ -2079,7 +2082,7 @@
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="B19">
         <v>2</v>
@@ -2087,7 +2090,7 @@
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="B20">
         <v>2</v>
@@ -2095,7 +2098,7 @@
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="B21">
         <v>2</v>
@@ -2103,7 +2106,7 @@
     </row>
     <row r="22" spans="1:2">
       <c r="A22" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="B22">
         <v>2</v>
@@ -2111,7 +2114,7 @@
     </row>
     <row r="23" spans="1:2">
       <c r="A23" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="B23">
         <v>2</v>
@@ -2119,7 +2122,7 @@
     </row>
     <row r="24" spans="1:2">
       <c r="A24" t="s">
-        <v>29</v>
+        <v>15</v>
       </c>
       <c r="B24">
         <v>2</v>
@@ -2132,7 +2135,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2159,15 +2162,23 @@
         <v>37</v>
       </c>
       <c r="B3">
-        <v>700</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>38</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
         <v>39</v>
+      </c>
+      <c r="B5" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Freeze excel header rows
</commit_message>
<xml_diff>
--- a/data/filtered.xlsx
+++ b/data/filtered.xlsx
@@ -498,7 +498,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
@@ -1932,7 +1935,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B24"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
@@ -2137,7 +2143,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>

</xml_diff>